<commit_message>
Add list inbound and outbound in Excel file
</commit_message>
<xml_diff>
--- a/Kohi/InboundImport.xlsx
+++ b/Kohi/InboundImport.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/30da737a58fca011/Máy tính/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kohi\Kohi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="8_{B84EA33D-1A77-4CEE-AD98-DC93A138EFC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{346FC9FB-9BA7-4A76-B668-CFF3871FBF4B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8247E37-C07C-41E0-A501-4368F44D84EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10276" xr2:uid="{4CFBD19E-7A84-4058-8D5B-29A880EB4F9B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>IngredientName</t>
   </si>
@@ -72,6 +72,12 @@
   </si>
   <si>
     <t>TeaFarm</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Tốt</t>
   </si>
 </sst>
 </file>
@@ -444,15 +450,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{290C02A0-A51E-4CE0-A2D8-6F278A861B50}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -471,8 +477,11 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -491,8 +500,11 @@
       <c r="F2" s="1">
         <v>46360</v>
       </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -511,8 +523,11 @@
       <c r="F3" s="1">
         <v>46360</v>
       </c>
+      <c r="G3" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -530,6 +545,9 @@
       </c>
       <c r="F4" s="1">
         <v>46360</v>
+      </c>
+      <c r="G4" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>